<commit_message>
Tested. Reverted to images on root.
</commit_message>
<xml_diff>
--- a/images.xlsx
+++ b/images.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tobii-my.sharepoint.com/personal/ao1733_tobii_com/Documents/Desktop/PsychoPy/EEG experiment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="11_D314AE8F02D700CD9DBCD4915F8BCCFB9B5C8421" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{180868A3-0E82-4E65-82E6-2A697453AFEB}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="11_B55CEF8DC2D600CD9DBCD4606F1D759F8378C492" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D085A515-247C-45C2-8B92-ABC04076CF16}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="450" yWindow="8640" windowWidth="26850" windowHeight="22755" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,9 +25,6 @@
     <t>images</t>
   </si>
   <si>
-    <t>level</t>
-  </si>
-  <si>
     <t>target_x</t>
   </si>
   <si>
@@ -40,22 +37,25 @@
     <t>high</t>
   </si>
   <si>
-    <t>data/img1.png</t>
-  </si>
-  <si>
-    <t>data/img2.png</t>
-  </si>
-  <si>
-    <t>data/img3.png</t>
-  </si>
-  <si>
-    <t>data/img4.png</t>
-  </si>
-  <si>
-    <t>data/img5.png</t>
-  </si>
-  <si>
-    <t>data/img6.png</t>
+    <t>img1.png</t>
+  </si>
+  <si>
+    <t>img2.png</t>
+  </si>
+  <si>
+    <t>img3.png</t>
+  </si>
+  <si>
+    <t>img4.png</t>
+  </si>
+  <si>
+    <t>img5.png</t>
+  </si>
+  <si>
+    <t>img6.png</t>
+  </si>
+  <si>
+    <t>diff_level</t>
   </si>
 </sst>
 </file>
@@ -72,7 +72,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -106,10 +106,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -420,110 +420,110 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="C2" s="1">
+        <v>-0.34875</v>
+      </c>
+      <c r="D2" s="1">
+        <v>-0.25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2">
-        <v>-0.34875</v>
-      </c>
-      <c r="D2" s="2">
-        <v>-0.25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="C3" s="1">
+        <v>0.19125</v>
+      </c>
+      <c r="D3" s="1">
+        <v>-0.44500000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="2">
-        <v>0.19125</v>
-      </c>
-      <c r="D3" s="2">
-        <v>-0.44500000000000001</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0.42249999999999999</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0.27374999999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>8</v>
       </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="2">
-        <v>0.42249999999999999</v>
-      </c>
-      <c r="D4" s="2">
-        <v>0.27374999999999999</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0.85958333333333303</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0.38333333333333303</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>9</v>
       </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="2">
-        <v>0.85958333333333303</v>
-      </c>
-      <c r="D5" s="2">
-        <v>0.38333333333333303</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0.24520833333333</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0.64520833333333305</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>10</v>
       </c>
-      <c r="B6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="2">
-        <v>0.24520833333333</v>
-      </c>
-      <c r="D6" s="2">
-        <v>0.64520833333333305</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>11</v>
-      </c>
       <c r="B7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="2">
+        <v>3</v>
+      </c>
+      <c r="C7" s="1">
         <v>0.63083333333333003</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="1">
         <v>0.90708333333333302</v>
       </c>
     </row>

</xml_diff>

<commit_message>
EEG trigger and AOI updates
Added EEG triggers based on diff_level, updated AOI co-ords
</commit_message>
<xml_diff>
--- a/images.xlsx
+++ b/images.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tobii-my.sharepoint.com/personal/ao1733_tobii_com/Documents/Desktop/PsychoPy/EEG experiment/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Downloads\eeg-experiment-main\eeg-experiment-main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="11_B55CEF8DC2D600CD9DBCD4606F1D759F8378C492" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D085A515-247C-45C2-8B92-ABC04076CF16}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{529CDFDA-F587-41EB-B0A6-D0170FC35C09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="450" yWindow="8640" windowWidth="26850" windowHeight="22755" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,6 +37,9 @@
     <t>high</t>
   </si>
   <si>
+    <t>diff_level</t>
+  </si>
+  <si>
     <t>img1.png</t>
   </si>
   <si>
@@ -53,28 +56,19 @@
   </si>
   <si>
     <t>img6.png</t>
-  </si>
-  <si>
-    <t>diff_level</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -85,14 +79,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -104,11 +91,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -420,21 +404,22 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.42578125" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -443,88 +428,88 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="1">
-        <v>-0.34875</v>
-      </c>
-      <c r="D2" s="1">
-        <v>-0.25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C2">
+        <v>0.16018518518518499</v>
+      </c>
+      <c r="D2">
+        <v>-0.43611111111111101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="1">
-        <v>0.19125</v>
-      </c>
-      <c r="D3" s="1">
-        <v>-0.44500000000000001</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C3">
+        <v>0.75833333333333297</v>
+      </c>
+      <c r="D3">
+        <v>-9.9074074074073995E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="1">
-        <v>0.42249999999999999</v>
-      </c>
-      <c r="D4" s="1">
-        <v>0.27374999999999999</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C4">
+        <v>0.42499999999999999</v>
+      </c>
+      <c r="D4">
+        <v>-0.20740740740740701</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="1">
-        <v>0.85958333333333303</v>
-      </c>
-      <c r="D5" s="1">
-        <v>0.38333333333333303</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5">
+        <v>-0.42777777777777698</v>
+      </c>
+      <c r="D5">
+        <v>-0.19166666666666601</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="1">
-        <v>0.24520833333333</v>
-      </c>
-      <c r="D6" s="1">
-        <v>0.64520833333333305</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <v>-0.50925925925925897</v>
+      </c>
+      <c r="D6">
+        <v>0.141666666666666</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="1">
-        <v>0.63083333333333003</v>
-      </c>
-      <c r="D7" s="1">
-        <v>0.90708333333333302</v>
+      <c r="C7">
+        <v>0.67592592592592504</v>
+      </c>
+      <c r="D7">
+        <v>0.29537037037037001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>